<commit_message>
add service specific & charging
</commit_message>
<xml_diff>
--- a/Data/Temp/Template.xlsx
+++ b/Data/Temp/Template.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Technical Information" sheetId="2" r:id="rId2"/>
     <sheet name="VAS" sheetId="6" r:id="rId3"/>
     <sheet name="Implement Flow &amp; Ttime Plan" sheetId="4" r:id="rId4"/>
+    <sheet name="Service Specification" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="232">
   <si>
     <t>Value</t>
   </si>
@@ -156,9 +157,6 @@
     <t>Tetative Launch</t>
   </si>
   <si>
-    <t>*3154750</t>
-  </si>
-  <si>
     <t>ipHyb</t>
   </si>
   <si>
@@ -544,6 +542,183 @@
   </si>
   <si>
     <t>BACKGROUND / WALL PAPER</t>
+  </si>
+  <si>
+    <t>*4154750</t>
+  </si>
+  <si>
+    <t>specific.</t>
+  </si>
+  <si>
+    <t>Charge Group 2</t>
+  </si>
+  <si>
+    <t>Charge Group 3</t>
+  </si>
+  <si>
+    <t>Charge Group 1</t>
+  </si>
+  <si>
+    <t>120RedCross Donation (Transaction)^บริจาคเงินสมทบโครงการ 120RedCross (ครั้ง)</t>
+  </si>
+  <si>
+    <t>BUG1113(SMS) (Transaction)^บริการ BUG1113 (SMS) (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Calling Gift Monthly Fee (Mobile)^ค่าบริการรายเดือน Calling Gift (เลขหมาย)</t>
+  </si>
+  <si>
+    <t>Calling Melody - Calling Gift (Transaction)^บริการเพลงรอสาย-ส่งเพลงรอสาย (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Calling Melody - Calling Station (Station)^บริการ Calling Melody - Calling Station (สถานี)</t>
+  </si>
+  <si>
+    <t>Calling Melody - Rental Song (Song)^บริการ Calling Melody - เช่าเพลงรายเดือน (เพลง)</t>
+  </si>
+  <si>
+    <t>Calling Melody -Song 's fee (Transaction)^บริการเลือกเพลง Calling Melody (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Calling Post -SMS update(Transaction)^คอลลิ่ง โพสต์-ค่าSMSเปลี่ยนข้อความ(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Donation (Transaction)^บริจาคช่วยเหลือผู้ประสบภัย (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Download/Live Match/Online Entertainment (Transaction)^บริการดาวน์โหลด/ถ่ายทอดสดบอล/ดูรายการบันเทิงออนไลน์ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Easy Code Marketing (Transaction)^บริการอีซี่โค้ดมาร์เกตติ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Easy Message Marketing (Transaction)^บริการอีซี่เมสเสจมาร์เกตติ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Email2Message (Transaction)^บริการอีเมล์ทูเมสเสจ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>GSM Top Up for Prepaid (VAT Included)^ค่าใช้บริการโทรศัพท์เคลื่อนที่แบบเติมเงินล่วงหน้า (รวมภาษีมูลค่าเพิ่ม)</t>
+  </si>
+  <si>
+    <t>selected="selected"&gt;Info/Entertainment SMS (Clip/Horo/News/Vote/Activities etc.)^บริการรับส่งSMSข้อมูล-บันเทิง เช่น คลิป/ดวง/ข่าว/ร่วมกิจกรรม</t>
+  </si>
+  <si>
+    <t>International Call Charges from previous bill cycle^ค่าบริการข้ามแดนอัตโนมัติรอบบิลก่อนหน้า</t>
+  </si>
+  <si>
+    <t>International Roaming Charges from previous bill cycle^ค่าโทรทางไกลระหว่างประเทศรอบบิลก่อนหน้า</t>
+  </si>
+  <si>
+    <t>Mao Mao Gift (Transaction)^เหมา เหมา กิฟต์ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mBanking (Transaction)^บริการเอ็มแบงก์กิ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mBroker (Transaction)^บริการเอ็มโบรกเกอร์ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mClose2Me (Transaction)^บริการสอบถามเส้นทางผ่านมือถือ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mMessaging (Transaction)^บริการเอ็มแมสเสจจิ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>MMS Song2U (Transaction)^MMS Song2U (ครั้ง)</t>
+  </si>
+  <si>
+    <t>MMS Transport (Transaction)^เอ็มเอ็มเอส ทรานสปอร์ต (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Mobile Lucky (Transaction)^กิจกรรมลุ้นรับของรางวัล (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Mobile Marketing : Digital Coupon (Transaction)^บริการโมบายมาร์เกตติ้งดิจิตอลคูปอง(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Mobile Marketing : Location (Transaction)^บริการโมบายมาร์เกตติ้งโลเคชั่น(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Mobile Marketing : Member (Transaction)^บริการโมบายมาร์เกตติ้งเมมเบอร์(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Mobile Tracking (Transaction)^บริการ โมบาย แทรคกิ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mShopping (Transaction)^บริการเอ็มชอปปิ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mTargeting Broadcasting (Transaction)^เอ็มทาร์เก็ตติ้งบรอดแคสติ้ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mTargeting Conditioning (Transaction)^เอ็มทาร์เก็ตติ้งคอนดิชั่นนิ่ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mTargeting Profiling (Transaction)^เอ็มทาร์เก็ตติ้งโปรไฟล์ลิ่ง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>mUp2Date (Transaction)^บริการรายงานความเคลื่อนไหวผ่านมือถือ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Music/VDO Clips/Movies/Games Download (Transaction)^โหลดVDOคลิป/เพลง/ภาพยนตร์/เกมส์ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>My Logo,My Ringtone (Transaction)^บริการมายโลโก้ มายริงโทน (ครั้ง)</t>
+  </si>
+  <si>
+    <t>News/Horo/Facebook/Info/Entertainment Pack (Transaction)^รับSMSข่าว/ดูดวง/เฟสบุ๊ก/สาระ/บันเทิง (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Package Fee (Pack)/eBook Download (Time)^ค่าแพ็กเกจ(แพ็ก)/โหลดหนังสือeBook(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Pictures/Wallpapers/Books Download (Transaction)^โหลดภาพ/วอลเปเปอร์/หนังสือ (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Replied MMS on Smart Messaging (MMS)^บริการ Reply MMS Smart Messaging (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Send-Receive USSD2USSD,USSD2SMS (Transaction)^บริการรับส่ง USSD2USSD,USSD2SMS (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Service fees for payment collection on behalf of third parties^ค่าสินค้าและบริการเรียกเก็บแทน</t>
+  </si>
+  <si>
+    <t>SIRIRAJ DONATION (Transaction)^บริจาคเพื่อโรงพยาบาลศิริราช (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Siriraj Hospital Donate *984# (Transaction)^โครงการทำดีได้ด้วยปลายนิ้ว รพ.ศิริราช (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Smart Cloud (licenses)^บริการสมาร์ท คลาวด์ (ไลเซ่นส์)</t>
+  </si>
+  <si>
+    <t>Smart USSD (Transaction)^บริการรับส่งข้อความ USSD (ครั้ง)</t>
+  </si>
+  <si>
+    <t>SMS (Transaction)^บริการรับส่งข้อความ SMS (ครั้ง)</t>
+  </si>
+  <si>
+    <t>SMS AIS Aunjai Dai Tam *544^ข้อความจาก เอไอเอส อุ่นใจ ได้แต้ม *544</t>
+  </si>
+  <si>
+    <t>Software Mall (Transaction)^Software Mall (ครั้ง)</t>
+  </si>
+  <si>
+    <t>The DOWN donation (transaction)^บริจาค The DOWNมอบให้สถาบันราชานุกูล(ครั้ง)</t>
+  </si>
+  <si>
+    <t>Votes/Quiz SMS/MMS (Transactions)^ส่งSMSโหวต/ตอบคำถามชิงรางวัล (ครั้ง)</t>
+  </si>
+  <si>
+    <t>Charge Group2</t>
+  </si>
+  <si>
+    <t>Charge Group1</t>
+  </si>
+  <si>
+    <t>Charge Group0</t>
   </si>
 </sst>
 </file>
@@ -553,7 +728,7 @@
   <numFmts count="1">
     <numFmt numFmtId="187" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -627,6 +802,12 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -771,7 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -964,6 +1145,9 @@
     </xf>
     <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -985,6 +1169,18 @@
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="99" dropStyle="combo" dx="16" fmlaLink="$I$8" fmlaRange="$H$9:$H$42" noThreeD="1" sel="30" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="99" dropStyle="combo" dx="16" fmlaLink="$I$8" fmlaRange="$H$9:$H$60" noThreeD="1" sel="2" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="99" dropStyle="combo" dx="16" fmlaLink="$K$8" fmlaRange="$J$9:$J$60" noThreeD="1" sel="20" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="99" dropStyle="combo" dx="16" fmlaLink="$M$8" fmlaRange="$L$9:$L$60" noThreeD="1" sel="17" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1578,6 +1774,176 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>6115050</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4097" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4097"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>6115050</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4100" name="Drop Down 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4100"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>6124575</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>285750</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4101" name="Drop Down 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s4101"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1879,7 +2245,7 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1934,7 +2300,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1">
@@ -1945,7 +2311,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="20.100000000000001" customHeight="1">
@@ -1967,8 +2333,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -2033,7 +2399,7 @@
         <v>test.ipAddr</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>5</v>
@@ -2061,10 +2427,10 @@
         <v>test.ipHyb</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>11</v>
@@ -2224,7 +2590,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A21 A12:A17 A3:A8">
       <formula1>"awdawd"</formula1>
     </dataValidation>
@@ -2302,7 +2668,7 @@
     </row>
     <row r="2" spans="1:29" ht="24.95" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="9" t="str">
         <f>A$7 &amp; "group"</f>
@@ -2320,7 +2686,7 @@
     </row>
     <row r="3" spans="1:29" ht="24.95" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="9" t="str">
         <f>A$7 &amp; "type"</f>
@@ -2363,7 +2729,7 @@
     </row>
     <row r="7" spans="1:29" ht="24.95" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H7" s="62"/>
       <c r="I7" s="52"/>
@@ -2374,13 +2740,13 @@
       <c r="B8" s="63"/>
       <c r="C8" s="60"/>
       <c r="H8" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" s="46">
         <v>30</v>
       </c>
       <c r="J8" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K8" s="62">
         <v>50</v>
@@ -2404,11 +2770,11 @@
       <c r="B10" s="63"/>
       <c r="C10" s="60"/>
       <c r="H10" s="52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K10" s="55"/>
     </row>
@@ -2416,11 +2782,11 @@
       <c r="B11" s="63"/>
       <c r="C11" s="60"/>
       <c r="H11" s="52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11" s="52"/>
       <c r="J11" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K11" s="55"/>
     </row>
@@ -2428,11 +2794,11 @@
       <c r="B12" s="63"/>
       <c r="C12" s="61"/>
       <c r="H12" s="52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="52"/>
       <c r="J12" s="53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K12" s="55"/>
     </row>
@@ -2440,11 +2806,11 @@
       <c r="B13" s="63"/>
       <c r="C13" s="61"/>
       <c r="H13" s="52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I13" s="52"/>
       <c r="J13" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K13" s="55"/>
     </row>
@@ -2452,11 +2818,11 @@
       <c r="B14" s="63"/>
       <c r="C14" s="61"/>
       <c r="H14" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="52"/>
       <c r="J14" s="55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K14" s="54"/>
     </row>
@@ -2464,11 +2830,11 @@
       <c r="B15" s="63"/>
       <c r="C15" s="61"/>
       <c r="H15" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="52"/>
       <c r="J15" s="55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K15" s="54"/>
     </row>
@@ -2476,447 +2842,447 @@
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="H16" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="52"/>
       <c r="J16" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="54"/>
     </row>
     <row r="17" spans="8:11" ht="24.95" customHeight="1">
       <c r="H17" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K17" s="54"/>
     </row>
     <row r="18" spans="8:11" ht="24.95" customHeight="1">
       <c r="H18" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J18" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K18" s="54"/>
     </row>
     <row r="19" spans="8:11" ht="24.95" customHeight="1">
       <c r="H19" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="8:11" ht="24.95" customHeight="1">
       <c r="H20" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J20" s="55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="8:11" ht="24.95" customHeight="1">
       <c r="H21" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J21" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="8:11" ht="24.95" customHeight="1">
       <c r="H22" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" s="55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="8:11" ht="24.95" customHeight="1">
       <c r="H23" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J23" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="8:11" ht="24.95" customHeight="1">
       <c r="H24" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J24" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="8:11" ht="24.95" customHeight="1">
       <c r="H25" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J25" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="8:11" ht="24.95" customHeight="1">
       <c r="H26" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J26" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="8:11" ht="24.95" customHeight="1">
       <c r="H27" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="8:11" ht="24.95" customHeight="1">
       <c r="H28" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J28" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="8:11" ht="24.95" customHeight="1">
       <c r="H29" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J29" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="8:11" ht="24.95" customHeight="1">
       <c r="H30" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J30" s="55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="8:11" ht="24.95" customHeight="1">
       <c r="H31" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="8:11" ht="24.95" customHeight="1">
       <c r="H32" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="8:10" ht="24.95" customHeight="1">
       <c r="H33" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J33" s="55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="8:10" ht="24.95" customHeight="1">
       <c r="H34" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="8:10" ht="24.95" customHeight="1">
       <c r="H35" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="8:10" ht="24.95" customHeight="1">
       <c r="H36" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="8:10" ht="24.95" customHeight="1">
       <c r="H37" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="8:10" ht="24.95" customHeight="1">
       <c r="H38" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="8:10" ht="24.95" customHeight="1">
       <c r="H39" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="8:10" ht="24.95" customHeight="1">
       <c r="H40" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="8:10" ht="24.95" customHeight="1">
       <c r="H41" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="8:10" ht="24.95" customHeight="1">
       <c r="H42" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="8:10" ht="24.95" customHeight="1">
       <c r="J43" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="8:10" ht="24.95" customHeight="1">
       <c r="J44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="8:10" ht="24.95" customHeight="1">
       <c r="J45" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="8:10" ht="24.95" customHeight="1">
       <c r="J46" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="8:10" ht="24.95" customHeight="1">
       <c r="J47" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="8:10" ht="24.95" customHeight="1">
       <c r="J48" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="10:10" ht="24.95" customHeight="1">
       <c r="J49" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="10:10" ht="24.95" customHeight="1">
       <c r="J50" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="10:10" ht="24.95" customHeight="1">
       <c r="J51" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="10:10" ht="24.95" customHeight="1">
       <c r="J52" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="10:10" ht="24.95" customHeight="1">
       <c r="J53" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="10:10" ht="24.95" customHeight="1">
       <c r="J54" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="10:10" ht="24.95" customHeight="1">
       <c r="J55" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="10:10" ht="24.95" customHeight="1">
       <c r="J56" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="10:10" ht="24.95" customHeight="1">
       <c r="J57" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="10:10" ht="24.95" customHeight="1">
       <c r="J58" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="10:10" ht="24.95" customHeight="1">
       <c r="J59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="10:10" ht="24.95" customHeight="1">
       <c r="J60" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="10:10" ht="24.95" customHeight="1">
       <c r="J61" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="10:10" ht="24.95" customHeight="1">
       <c r="J62" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="10:10" ht="24.95" customHeight="1">
       <c r="J63" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="10:10" ht="24.95" customHeight="1">
       <c r="J64" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="10:10" ht="24.95" customHeight="1">
       <c r="J65" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="10:10" ht="24.95" customHeight="1">
       <c r="J66" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="10:10" ht="24.95" customHeight="1">
       <c r="J67" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="10:10" ht="24.95" customHeight="1">
       <c r="J68" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="10:10" ht="24.95" customHeight="1">
       <c r="J69" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="10:10" ht="24.95" customHeight="1">
       <c r="J70" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="10:10" ht="24.95" customHeight="1">
       <c r="J71" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="10:10" ht="24.95" customHeight="1">
       <c r="J72" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="10:10" ht="24.95" customHeight="1">
       <c r="J73" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="10:10" ht="24.95" customHeight="1">
       <c r="J74" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="10:10" ht="24.95" customHeight="1">
       <c r="J75" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="10:10" ht="24.95" customHeight="1">
       <c r="J76" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="10:10" ht="24.95" customHeight="1">
       <c r="J77" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="10:10" ht="24.95" customHeight="1">
       <c r="J78" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="10:10" ht="24.95" customHeight="1">
       <c r="J79" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="10:10" ht="24.95" customHeight="1">
       <c r="J80" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="10:10" ht="24.95" customHeight="1">
       <c r="J81" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="10:10" ht="24.95" customHeight="1">
       <c r="J82" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="10:10" ht="24.95" customHeight="1">
       <c r="J83" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="10:10" ht="24.95" customHeight="1">
       <c r="J84" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="10:10" ht="24.95" customHeight="1">
       <c r="J85" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="10:10" ht="24.95" customHeight="1">
       <c r="J86" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="10:10" ht="24.95" customHeight="1">
       <c r="J87" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +3349,7 @@
   <dimension ref="A1:AC39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="24.95" customHeight="1"/>
@@ -3169,16 +3535,16 @@
         <v>imple.tetative</v>
       </c>
       <c r="C8" s="27">
-        <v>43853</v>
+        <v>43839</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="49">
         <v>5</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="47">
         <v>4</v>
@@ -3194,16 +3560,16 @@
         <v>imple.commercial</v>
       </c>
       <c r="C9" s="27">
-        <v>43839</v>
+        <v>43840</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="49">
         <v>6</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="47">
         <v>5</v>
@@ -3235,16 +3601,16 @@
         <v>39</v>
       </c>
       <c r="H13" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I13" s="51">
         <v>1</v>
       </c>
       <c r="J13" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="50" t="s">
         <v>53</v>
-      </c>
-      <c r="K13" s="50" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="24.95" customHeight="1">
@@ -3257,16 +3623,16 @@
         <v>43832</v>
       </c>
       <c r="H14" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="46">
         <v>2</v>
       </c>
       <c r="J14" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="50" t="s">
         <v>55</v>
-      </c>
-      <c r="K14" s="50" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="24.95" customHeight="1">
@@ -3285,10 +3651,10 @@
       </c>
       <c r="I15" s="21"/>
       <c r="J15" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K15" s="55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="24.95" customHeight="1">
@@ -3305,10 +3671,10 @@
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K16" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="24.95" customHeight="1">
@@ -3325,10 +3691,10 @@
       </c>
       <c r="I17" s="52"/>
       <c r="J17" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K17" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="24.95" customHeight="1">
@@ -3345,10 +3711,10 @@
       </c>
       <c r="I18" s="52"/>
       <c r="J18" s="53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K18" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="24.95" customHeight="1">
@@ -3365,10 +3731,10 @@
       </c>
       <c r="I19" s="52"/>
       <c r="J19" s="55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K19" s="55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="24.95" customHeight="1">
@@ -3385,7 +3751,7 @@
       </c>
       <c r="I20" s="52"/>
       <c r="J20" s="55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K20" s="54"/>
     </row>
@@ -3403,7 +3769,7 @@
       </c>
       <c r="I21" s="52"/>
       <c r="J21" s="55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K21" s="54"/>
     </row>
@@ -3413,25 +3779,25 @@
       </c>
       <c r="I22" s="52"/>
       <c r="J22" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K22" s="54"/>
     </row>
     <row r="23" spans="2:11" ht="24.95" customHeight="1">
       <c r="J23" s="55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K23" s="54"/>
     </row>
     <row r="24" spans="2:11" ht="24.95" customHeight="1">
       <c r="J24" s="55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K24" s="54"/>
     </row>
     <row r="25" spans="2:11" ht="24.95" customHeight="1">
       <c r="J25" s="55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="24.95" customHeight="1">
@@ -3678,4 +4044,862 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="24.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="97.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="61.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="42.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" style="2" customWidth="1"/>
+    <col min="14" max="29" width="8.7109375" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="14.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="24.95" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
+      <c r="J1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="24.95" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="9" t="str">
+        <f>A$7 &amp; "chargeGroup1"</f>
+        <v>specific.chargeGroup1</v>
+      </c>
+      <c r="C2" s="44" t="str">
+        <f ca="1">INDIRECT("H" &amp; 8 + (I8))</f>
+        <v>120RedCross Donation (Transaction)^บริจาคเงินสมทบโครงการ 120RedCross (ครั้ง)</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="30"/>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="1:29" ht="24.95" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="9" t="str">
+        <f>A$7 &amp; "chargeGroup2"</f>
+        <v>specific.chargeGroup2</v>
+      </c>
+      <c r="C3" s="28" t="str">
+        <f ca="1">INDIRECT("J" &amp; 8 + (K8))</f>
+        <v>mBanking (Transaction)^บริการเอ็มแบงก์กิ้ง (ครั้ง)</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="30"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="1:29" ht="24.95" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="9" t="str">
+        <f>A$7 &amp; "chargeGroup3"</f>
+        <v>specific.chargeGroup3</v>
+      </c>
+      <c r="C4" s="28" t="str">
+        <f ca="1">INDIRECT("L" &amp; 8 + (M8))</f>
+        <v>International Call Charges from previous bill cycle^ค่าบริการข้ามแดนอัตโนมัติรอบบิลก่อนหน้า</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:29" ht="24.95" customHeight="1">
+      <c r="C5" s="3"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:29" ht="24.95" customHeight="1">
+      <c r="E6" s="43"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:29" ht="24.95" customHeight="1">
+      <c r="A7" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="62"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+    </row>
+    <row r="8" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B8" s="63"/>
+      <c r="C8" s="60"/>
+      <c r="H8" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="I8" s="46">
+        <v>2</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="K8" s="46">
+        <v>20</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="M8" s="46">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B9" s="63"/>
+      <c r="C9" s="60"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="21"/>
+    </row>
+    <row r="10" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B10" s="63"/>
+      <c r="C10" s="60"/>
+      <c r="H10" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="K10" s="21"/>
+      <c r="L10" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="21"/>
+    </row>
+    <row r="11" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B11" s="63"/>
+      <c r="C11" s="60"/>
+      <c r="H11" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="I11" s="52"/>
+      <c r="J11" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="K11" s="52"/>
+      <c r="L11" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="52"/>
+    </row>
+    <row r="12" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B12" s="63"/>
+      <c r="C12" s="61"/>
+      <c r="H12" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="I12" s="52"/>
+      <c r="J12" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="K12" s="52"/>
+      <c r="L12" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="M12" s="52"/>
+    </row>
+    <row r="13" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B13" s="63"/>
+      <c r="C13" s="61"/>
+      <c r="H13" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="52"/>
+      <c r="J13" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" s="52"/>
+      <c r="L13" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" s="52"/>
+    </row>
+    <row r="14" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B14" s="63"/>
+      <c r="C14" s="61"/>
+      <c r="H14" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="52"/>
+      <c r="J14" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="K14" s="52"/>
+      <c r="L14" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="M14" s="52"/>
+    </row>
+    <row r="15" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B15" s="63"/>
+      <c r="C15" s="61"/>
+      <c r="H15" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="K15" s="52"/>
+      <c r="L15" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="M15" s="52"/>
+    </row>
+    <row r="16" spans="1:29" ht="24.95" customHeight="1">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="H16" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" s="52"/>
+      <c r="J16" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="K16" s="52"/>
+      <c r="L16" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="M16" s="52"/>
+    </row>
+    <row r="17" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H17" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="L17" s="65" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H18" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H19" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="L19" s="65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H20" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="L20" s="65" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H21" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="J21" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="L21" s="65" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H22" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="J22" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="L22" s="65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H23" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="J23" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="L23" s="65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H24" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="J24" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="L24" s="65" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H25" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="J25" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="L25" s="65" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H26" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="L26" s="65" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H27" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="J27" s="65" t="s">
+        <v>195</v>
+      </c>
+      <c r="L27" s="65" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H28" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="J28" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="L28" s="65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H29" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="J29" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="L29" s="65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H30" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="J30" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="L30" s="65" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H31" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="J31" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="L31" s="65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H32" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="J32" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="L32" s="65" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H33" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="J33" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="L33" s="65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H34" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="J34" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="L34" s="65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H35" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="J35" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="L35" s="65" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H36" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="J36" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="L36" s="65" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H37" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="J37" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="L37" s="65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H38" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="J38" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="L38" s="65" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H39" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="J39" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="L39" s="65" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H40" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="J40" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="L40" s="65" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H41" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="J41" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="L41" s="65" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H42" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="J42" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="L42" s="65" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H43" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="J43" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="L43" s="65" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H44" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="J44" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="L44" s="65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H45" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="J45" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="L45" s="65" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H46" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="J46" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="L46" s="65" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H47" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="J47" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="L47" s="65" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="48" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H48" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="J48" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="L48" s="65" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H49" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="J49" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="L49" s="65" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H50" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="J50" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="L50" s="65" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H51" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="J51" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="L51" s="65" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H52" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="J52" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="L52" s="65" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H53" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="J53" s="65" t="s">
+        <v>221</v>
+      </c>
+      <c r="L53" s="65" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H54" s="65" t="s">
+        <v>222</v>
+      </c>
+      <c r="J54" s="65" t="s">
+        <v>222</v>
+      </c>
+      <c r="L54" s="65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H55" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="J55" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="L55" s="65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H56" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="J56" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="L56" s="65" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H57" s="65" t="s">
+        <v>225</v>
+      </c>
+      <c r="J57" s="65" t="s">
+        <v>225</v>
+      </c>
+      <c r="L57" s="65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H58" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="J58" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="L58" s="65" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H59" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="J59" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="L59" s="65" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="8:12" ht="24.95" customHeight="1">
+      <c r="H60" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="J60" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="L60" s="65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4097" r:id="rId4" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>6115050</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4100" r:id="rId5" name="Drop Down 4">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>6115050</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="4101" r:id="rId6" name="Drop Down 5">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>381000</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>6124575</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>285750</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>